<commit_message>
add example terms to plant growth related templates
</commit_message>
<xml_diff>
--- a/templates/dataplant/Plant_growth_conditions.xlsx
+++ b/templates/dataplant/Plant_growth_conditions.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="147">
   <si>
     <t>TEMPLATE</t>
   </si>
@@ -359,27 +359,60 @@
     <t>plant-growth.txt</t>
   </si>
   <si>
-    <t>A. thaliana</t>
-  </si>
-  <si>
-    <t>user-specific</t>
-  </si>
-  <si>
-    <t>field</t>
+    <t>Zea mays</t>
+  </si>
+  <si>
+    <t>NCBITaxon</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCBITaxon_4577</t>
+  </si>
+  <si>
+    <t>wild type genotype</t>
+  </si>
+  <si>
+    <t>EFO</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EFO_0005168</t>
+  </si>
+  <si>
+    <t>greenhouse study</t>
+  </si>
+  <si>
+    <t>PECO</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/PECO_0007248</t>
+  </si>
+  <si>
+    <t>20.04.2024</t>
+  </si>
+  <si>
+    <t>randomized complete block design</t>
+  </si>
+  <si>
+    <t>OBI</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0500007</t>
+  </si>
+  <si>
+    <t>soil</t>
   </si>
   <si>
     <t>ENVO</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/ENVO_01000352</t>
-  </si>
-  <si>
-    <t>soil</t>
-  </si>
-  <si>
     <t>http://purl.obolibrary.org/obo/ENVO_00001998</t>
   </si>
   <si>
+    <t>16 h</t>
+  </si>
+  <si>
+    <t>600</t>
+  </si>
+  <si>
     <t>microeinstein per square meter per second</t>
   </si>
   <si>
@@ -389,31 +422,37 @@
     <t>http://purl.obolibrary.org/obo/UO_0000160</t>
   </si>
   <si>
+    <t>50</t>
+  </si>
+  <si>
     <t>percent</t>
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/UO_0000187</t>
   </si>
   <si>
-    <t>Z. mays</t>
-  </si>
-  <si>
-    <t>Climate chamber</t>
-  </si>
-  <si>
-    <t>Hydroponic</t>
-  </si>
-  <si>
-    <t>Green house</t>
-  </si>
-  <si>
-    <t>agar</t>
-  </si>
-  <si>
-    <t>CHEBI</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/CHEBI_2509</t>
+    <t>25 °C</t>
+  </si>
+  <si>
+    <t>20 °C</t>
+  </si>
+  <si>
+    <t>70 % soil water content</t>
+  </si>
+  <si>
+    <t>nitrogen fertilizer exposure</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/PECO_0007102</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>Fusarium exposure</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/PECO_0007341</t>
   </si>
 </sst>
 </file>
@@ -469,8 +508,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" name="annotationTable" displayName="annotationTable" ref="A1:BE7" totalsRowShown="1" headerRowCount="1">
-  <autoFilter ref="A1:BE7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" name="annotationTable" displayName="annotationTable" ref="A1:BE2" totalsRowShown="1" headerRowCount="1">
+  <autoFilter ref="A1:BE2">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -1113,7 +1152,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BE7"/>
+  <dimension ref="A1:BE2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:57" x14ac:dyDescent="0.25">
@@ -1312,28 +1351,28 @@
         <v>116</v>
       </c>
       <c r="H2" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="I2" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="J2" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="K2" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="L2" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="M2" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="N2" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="O2" t="s">
-        <v>110</v>
+        <v>124</v>
       </c>
       <c r="P2" t="s">
         <v>110</v>
@@ -1342,25 +1381,25 @@
         <v>110</v>
       </c>
       <c r="R2" t="s">
-        <v>110</v>
+        <v>125</v>
       </c>
       <c r="S2" t="s">
-        <v>110</v>
+        <v>126</v>
       </c>
       <c r="T2" t="s">
-        <v>110</v>
+        <v>127</v>
       </c>
       <c r="U2" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="V2" t="s">
-        <v>118</v>
+        <v>129</v>
       </c>
       <c r="W2" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="X2" t="s">
-        <v>110</v>
+        <v>131</v>
       </c>
       <c r="Y2" t="s">
         <v>110</v>
@@ -1369,43 +1408,43 @@
         <v>110</v>
       </c>
       <c r="AA2" t="s">
-        <v>110</v>
+        <v>132</v>
       </c>
       <c r="AB2" t="s">
-        <v>122</v>
+        <v>133</v>
       </c>
       <c r="AC2" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
       <c r="AD2" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="AE2" t="s">
-        <v>110</v>
+        <v>136</v>
       </c>
       <c r="AF2" t="s">
-        <v>125</v>
+        <v>137</v>
       </c>
       <c r="AG2" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
       <c r="AH2" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
       <c r="AI2" t="s">
-        <v>110</v>
+        <v>136</v>
       </c>
       <c r="AJ2" t="s">
-        <v>125</v>
+        <v>137</v>
       </c>
       <c r="AK2" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
       <c r="AL2" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
       <c r="AM2" t="s">
-        <v>110</v>
+        <v>139</v>
       </c>
       <c r="AN2" t="s">
         <v>110</v>
@@ -1414,7 +1453,7 @@
         <v>110</v>
       </c>
       <c r="AP2" t="s">
-        <v>110</v>
+        <v>140</v>
       </c>
       <c r="AQ2" t="s">
         <v>110</v>
@@ -1423,7 +1462,7 @@
         <v>110</v>
       </c>
       <c r="AS2" t="s">
-        <v>110</v>
+        <v>141</v>
       </c>
       <c r="AT2" t="s">
         <v>110</v>
@@ -1432,16 +1471,16 @@
         <v>110</v>
       </c>
       <c r="AV2" t="s">
-        <v>110</v>
+        <v>142</v>
       </c>
       <c r="AW2" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
       <c r="AX2" t="s">
-        <v>110</v>
+        <v>143</v>
       </c>
       <c r="AY2" t="s">
-        <v>110</v>
+        <v>144</v>
       </c>
       <c r="AZ2" t="s">
         <v>110</v>
@@ -1450,880 +1489,15 @@
         <v>110</v>
       </c>
       <c r="BB2" t="s">
-        <v>110</v>
+        <v>145</v>
       </c>
       <c r="BC2" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
       <c r="BD2" t="s">
-        <v>110</v>
+        <v>146</v>
       </c>
       <c r="BE2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="3" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>110</v>
-      </c>
-      <c r="B3" t="s">
-        <v>111</v>
-      </c>
-      <c r="C3" t="s">
-        <v>112</v>
-      </c>
-      <c r="D3" t="s">
-        <v>113</v>
-      </c>
-      <c r="E3" t="s">
-        <v>114</v>
-      </c>
-      <c r="F3" t="s">
-        <v>127</v>
-      </c>
-      <c r="G3" t="s">
-        <v>116</v>
-      </c>
-      <c r="H3" t="s">
-        <v>110</v>
-      </c>
-      <c r="I3" t="s">
-        <v>110</v>
-      </c>
-      <c r="J3" t="s">
-        <v>110</v>
-      </c>
-      <c r="K3" t="s">
-        <v>110</v>
-      </c>
-      <c r="L3" t="s">
-        <v>128</v>
-      </c>
-      <c r="M3" t="s">
-        <v>116</v>
-      </c>
-      <c r="N3" t="s">
-        <v>110</v>
-      </c>
-      <c r="O3" t="s">
-        <v>110</v>
-      </c>
-      <c r="P3" t="s">
-        <v>110</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>110</v>
-      </c>
-      <c r="R3" t="s">
-        <v>110</v>
-      </c>
-      <c r="S3" t="s">
-        <v>110</v>
-      </c>
-      <c r="T3" t="s">
-        <v>110</v>
-      </c>
-      <c r="U3" t="s">
-        <v>129</v>
-      </c>
-      <c r="V3" t="s">
-        <v>116</v>
-      </c>
-      <c r="W3" t="s">
-        <v>110</v>
-      </c>
-      <c r="X3" t="s">
-        <v>110</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>110</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>110</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>110</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>122</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>123</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>124</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>110</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>110</v>
-      </c>
-      <c r="AG3" t="s">
-        <v>110</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>110</v>
-      </c>
-      <c r="AI3" t="s">
-        <v>110</v>
-      </c>
-      <c r="AJ3" t="s">
-        <v>110</v>
-      </c>
-      <c r="AK3" t="s">
-        <v>110</v>
-      </c>
-      <c r="AL3" t="s">
-        <v>110</v>
-      </c>
-      <c r="AM3" t="s">
-        <v>110</v>
-      </c>
-      <c r="AN3" t="s">
-        <v>110</v>
-      </c>
-      <c r="AO3" t="s">
-        <v>110</v>
-      </c>
-      <c r="AP3" t="s">
-        <v>110</v>
-      </c>
-      <c r="AQ3" t="s">
-        <v>110</v>
-      </c>
-      <c r="AR3" t="s">
-        <v>110</v>
-      </c>
-      <c r="AS3" t="s">
-        <v>110</v>
-      </c>
-      <c r="AT3" t="s">
-        <v>110</v>
-      </c>
-      <c r="AU3" t="s">
-        <v>110</v>
-      </c>
-      <c r="AV3" t="s">
-        <v>110</v>
-      </c>
-      <c r="AW3" t="s">
-        <v>110</v>
-      </c>
-      <c r="AX3" t="s">
-        <v>110</v>
-      </c>
-      <c r="AY3" t="s">
-        <v>110</v>
-      </c>
-      <c r="AZ3" t="s">
-        <v>110</v>
-      </c>
-      <c r="BA3" t="s">
-        <v>110</v>
-      </c>
-      <c r="BB3" t="s">
-        <v>110</v>
-      </c>
-      <c r="BC3" t="s">
-        <v>110</v>
-      </c>
-      <c r="BD3" t="s">
-        <v>110</v>
-      </c>
-      <c r="BE3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="4" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>110</v>
-      </c>
-      <c r="B4" t="s">
-        <v>111</v>
-      </c>
-      <c r="C4" t="s">
-        <v>112</v>
-      </c>
-      <c r="D4" t="s">
-        <v>113</v>
-      </c>
-      <c r="E4" t="s">
-        <v>114</v>
-      </c>
-      <c r="F4" t="s">
-        <v>110</v>
-      </c>
-      <c r="G4" t="s">
-        <v>110</v>
-      </c>
-      <c r="H4" t="s">
-        <v>110</v>
-      </c>
-      <c r="I4" t="s">
-        <v>110</v>
-      </c>
-      <c r="J4" t="s">
-        <v>110</v>
-      </c>
-      <c r="K4" t="s">
-        <v>110</v>
-      </c>
-      <c r="L4" t="s">
-        <v>130</v>
-      </c>
-      <c r="M4" t="s">
-        <v>116</v>
-      </c>
-      <c r="N4" t="s">
-        <v>110</v>
-      </c>
-      <c r="O4" t="s">
-        <v>110</v>
-      </c>
-      <c r="P4" t="s">
-        <v>110</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>110</v>
-      </c>
-      <c r="R4" t="s">
-        <v>110</v>
-      </c>
-      <c r="S4" t="s">
-        <v>110</v>
-      </c>
-      <c r="T4" t="s">
-        <v>110</v>
-      </c>
-      <c r="U4" t="s">
-        <v>131</v>
-      </c>
-      <c r="V4" t="s">
-        <v>132</v>
-      </c>
-      <c r="W4" t="s">
-        <v>133</v>
-      </c>
-      <c r="X4" t="s">
-        <v>110</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>110</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>110</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>110</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>122</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>123</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>124</v>
-      </c>
-      <c r="AE4" t="s">
-        <v>110</v>
-      </c>
-      <c r="AF4" t="s">
-        <v>110</v>
-      </c>
-      <c r="AG4" t="s">
-        <v>110</v>
-      </c>
-      <c r="AH4" t="s">
-        <v>110</v>
-      </c>
-      <c r="AI4" t="s">
-        <v>110</v>
-      </c>
-      <c r="AJ4" t="s">
-        <v>110</v>
-      </c>
-      <c r="AK4" t="s">
-        <v>110</v>
-      </c>
-      <c r="AL4" t="s">
-        <v>110</v>
-      </c>
-      <c r="AM4" t="s">
-        <v>110</v>
-      </c>
-      <c r="AN4" t="s">
-        <v>110</v>
-      </c>
-      <c r="AO4" t="s">
-        <v>110</v>
-      </c>
-      <c r="AP4" t="s">
-        <v>110</v>
-      </c>
-      <c r="AQ4" t="s">
-        <v>110</v>
-      </c>
-      <c r="AR4" t="s">
-        <v>110</v>
-      </c>
-      <c r="AS4" t="s">
-        <v>110</v>
-      </c>
-      <c r="AT4" t="s">
-        <v>110</v>
-      </c>
-      <c r="AU4" t="s">
-        <v>110</v>
-      </c>
-      <c r="AV4" t="s">
-        <v>110</v>
-      </c>
-      <c r="AW4" t="s">
-        <v>110</v>
-      </c>
-      <c r="AX4" t="s">
-        <v>110</v>
-      </c>
-      <c r="AY4" t="s">
-        <v>110</v>
-      </c>
-      <c r="AZ4" t="s">
-        <v>110</v>
-      </c>
-      <c r="BA4" t="s">
-        <v>110</v>
-      </c>
-      <c r="BB4" t="s">
-        <v>110</v>
-      </c>
-      <c r="BC4" t="s">
-        <v>110</v>
-      </c>
-      <c r="BD4" t="s">
-        <v>110</v>
-      </c>
-      <c r="BE4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="5" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>110</v>
-      </c>
-      <c r="B5" t="s">
-        <v>111</v>
-      </c>
-      <c r="C5" t="s">
-        <v>112</v>
-      </c>
-      <c r="D5" t="s">
-        <v>113</v>
-      </c>
-      <c r="E5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F5" t="s">
-        <v>110</v>
-      </c>
-      <c r="G5" t="s">
-        <v>110</v>
-      </c>
-      <c r="H5" t="s">
-        <v>110</v>
-      </c>
-      <c r="I5" t="s">
-        <v>110</v>
-      </c>
-      <c r="J5" t="s">
-        <v>110</v>
-      </c>
-      <c r="K5" t="s">
-        <v>110</v>
-      </c>
-      <c r="L5" t="s">
-        <v>110</v>
-      </c>
-      <c r="M5" t="s">
-        <v>110</v>
-      </c>
-      <c r="N5" t="s">
-        <v>110</v>
-      </c>
-      <c r="O5" t="s">
-        <v>110</v>
-      </c>
-      <c r="P5" t="s">
-        <v>110</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>110</v>
-      </c>
-      <c r="R5" t="s">
-        <v>110</v>
-      </c>
-      <c r="S5" t="s">
-        <v>110</v>
-      </c>
-      <c r="T5" t="s">
-        <v>110</v>
-      </c>
-      <c r="U5" t="s">
-        <v>110</v>
-      </c>
-      <c r="V5" t="s">
-        <v>110</v>
-      </c>
-      <c r="W5" t="s">
-        <v>110</v>
-      </c>
-      <c r="X5" t="s">
-        <v>110</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>110</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>110</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>110</v>
-      </c>
-      <c r="AB5" t="s">
-        <v>122</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>123</v>
-      </c>
-      <c r="AD5" t="s">
-        <v>124</v>
-      </c>
-      <c r="AE5" t="s">
-        <v>110</v>
-      </c>
-      <c r="AF5" t="s">
-        <v>110</v>
-      </c>
-      <c r="AG5" t="s">
-        <v>110</v>
-      </c>
-      <c r="AH5" t="s">
-        <v>110</v>
-      </c>
-      <c r="AI5" t="s">
-        <v>110</v>
-      </c>
-      <c r="AJ5" t="s">
-        <v>110</v>
-      </c>
-      <c r="AK5" t="s">
-        <v>110</v>
-      </c>
-      <c r="AL5" t="s">
-        <v>110</v>
-      </c>
-      <c r="AM5" t="s">
-        <v>110</v>
-      </c>
-      <c r="AN5" t="s">
-        <v>110</v>
-      </c>
-      <c r="AO5" t="s">
-        <v>110</v>
-      </c>
-      <c r="AP5" t="s">
-        <v>110</v>
-      </c>
-      <c r="AQ5" t="s">
-        <v>110</v>
-      </c>
-      <c r="AR5" t="s">
-        <v>110</v>
-      </c>
-      <c r="AS5" t="s">
-        <v>110</v>
-      </c>
-      <c r="AT5" t="s">
-        <v>110</v>
-      </c>
-      <c r="AU5" t="s">
-        <v>110</v>
-      </c>
-      <c r="AV5" t="s">
-        <v>110</v>
-      </c>
-      <c r="AW5" t="s">
-        <v>110</v>
-      </c>
-      <c r="AX5" t="s">
-        <v>110</v>
-      </c>
-      <c r="AY5" t="s">
-        <v>110</v>
-      </c>
-      <c r="AZ5" t="s">
-        <v>110</v>
-      </c>
-      <c r="BA5" t="s">
-        <v>110</v>
-      </c>
-      <c r="BB5" t="s">
-        <v>110</v>
-      </c>
-      <c r="BC5" t="s">
-        <v>110</v>
-      </c>
-      <c r="BD5" t="s">
-        <v>110</v>
-      </c>
-      <c r="BE5" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="6" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>110</v>
-      </c>
-      <c r="B6" t="s">
-        <v>111</v>
-      </c>
-      <c r="C6" t="s">
-        <v>112</v>
-      </c>
-      <c r="D6" t="s">
-        <v>113</v>
-      </c>
-      <c r="E6" t="s">
-        <v>114</v>
-      </c>
-      <c r="F6" t="s">
-        <v>110</v>
-      </c>
-      <c r="G6" t="s">
-        <v>110</v>
-      </c>
-      <c r="H6" t="s">
-        <v>110</v>
-      </c>
-      <c r="I6" t="s">
-        <v>110</v>
-      </c>
-      <c r="J6" t="s">
-        <v>110</v>
-      </c>
-      <c r="K6" t="s">
-        <v>110</v>
-      </c>
-      <c r="L6" t="s">
-        <v>110</v>
-      </c>
-      <c r="M6" t="s">
-        <v>110</v>
-      </c>
-      <c r="N6" t="s">
-        <v>110</v>
-      </c>
-      <c r="O6" t="s">
-        <v>110</v>
-      </c>
-      <c r="P6" t="s">
-        <v>110</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>110</v>
-      </c>
-      <c r="R6" t="s">
-        <v>110</v>
-      </c>
-      <c r="S6" t="s">
-        <v>110</v>
-      </c>
-      <c r="T6" t="s">
-        <v>110</v>
-      </c>
-      <c r="U6" t="s">
-        <v>110</v>
-      </c>
-      <c r="V6" t="s">
-        <v>110</v>
-      </c>
-      <c r="W6" t="s">
-        <v>110</v>
-      </c>
-      <c r="X6" t="s">
-        <v>110</v>
-      </c>
-      <c r="Y6" t="s">
-        <v>110</v>
-      </c>
-      <c r="Z6" t="s">
-        <v>110</v>
-      </c>
-      <c r="AA6" t="s">
-        <v>110</v>
-      </c>
-      <c r="AB6" t="s">
-        <v>122</v>
-      </c>
-      <c r="AC6" t="s">
-        <v>123</v>
-      </c>
-      <c r="AD6" t="s">
-        <v>124</v>
-      </c>
-      <c r="AE6" t="s">
-        <v>110</v>
-      </c>
-      <c r="AF6" t="s">
-        <v>110</v>
-      </c>
-      <c r="AG6" t="s">
-        <v>110</v>
-      </c>
-      <c r="AH6" t="s">
-        <v>110</v>
-      </c>
-      <c r="AI6" t="s">
-        <v>110</v>
-      </c>
-      <c r="AJ6" t="s">
-        <v>110</v>
-      </c>
-      <c r="AK6" t="s">
-        <v>110</v>
-      </c>
-      <c r="AL6" t="s">
-        <v>110</v>
-      </c>
-      <c r="AM6" t="s">
-        <v>110</v>
-      </c>
-      <c r="AN6" t="s">
-        <v>110</v>
-      </c>
-      <c r="AO6" t="s">
-        <v>110</v>
-      </c>
-      <c r="AP6" t="s">
-        <v>110</v>
-      </c>
-      <c r="AQ6" t="s">
-        <v>110</v>
-      </c>
-      <c r="AR6" t="s">
-        <v>110</v>
-      </c>
-      <c r="AS6" t="s">
-        <v>110</v>
-      </c>
-      <c r="AT6" t="s">
-        <v>110</v>
-      </c>
-      <c r="AU6" t="s">
-        <v>110</v>
-      </c>
-      <c r="AV6" t="s">
-        <v>110</v>
-      </c>
-      <c r="AW6" t="s">
-        <v>110</v>
-      </c>
-      <c r="AX6" t="s">
-        <v>110</v>
-      </c>
-      <c r="AY6" t="s">
-        <v>110</v>
-      </c>
-      <c r="AZ6" t="s">
-        <v>110</v>
-      </c>
-      <c r="BA6" t="s">
-        <v>110</v>
-      </c>
-      <c r="BB6" t="s">
-        <v>110</v>
-      </c>
-      <c r="BC6" t="s">
-        <v>110</v>
-      </c>
-      <c r="BD6" t="s">
-        <v>110</v>
-      </c>
-      <c r="BE6" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="7" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>110</v>
-      </c>
-      <c r="B7" t="s">
-        <v>111</v>
-      </c>
-      <c r="C7" t="s">
-        <v>112</v>
-      </c>
-      <c r="D7" t="s">
-        <v>113</v>
-      </c>
-      <c r="E7" t="s">
-        <v>114</v>
-      </c>
-      <c r="F7" t="s">
-        <v>110</v>
-      </c>
-      <c r="G7" t="s">
-        <v>110</v>
-      </c>
-      <c r="H7" t="s">
-        <v>110</v>
-      </c>
-      <c r="I7" t="s">
-        <v>110</v>
-      </c>
-      <c r="J7" t="s">
-        <v>110</v>
-      </c>
-      <c r="K7" t="s">
-        <v>110</v>
-      </c>
-      <c r="L7" t="s">
-        <v>110</v>
-      </c>
-      <c r="M7" t="s">
-        <v>110</v>
-      </c>
-      <c r="N7" t="s">
-        <v>110</v>
-      </c>
-      <c r="O7" t="s">
-        <v>110</v>
-      </c>
-      <c r="P7" t="s">
-        <v>110</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>110</v>
-      </c>
-      <c r="R7" t="s">
-        <v>110</v>
-      </c>
-      <c r="S7" t="s">
-        <v>110</v>
-      </c>
-      <c r="T7" t="s">
-        <v>110</v>
-      </c>
-      <c r="U7" t="s">
-        <v>110</v>
-      </c>
-      <c r="V7" t="s">
-        <v>110</v>
-      </c>
-      <c r="W7" t="s">
-        <v>110</v>
-      </c>
-      <c r="X7" t="s">
-        <v>110</v>
-      </c>
-      <c r="Y7" t="s">
-        <v>110</v>
-      </c>
-      <c r="Z7" t="s">
-        <v>110</v>
-      </c>
-      <c r="AA7" t="s">
-        <v>110</v>
-      </c>
-      <c r="AB7" t="s">
-        <v>122</v>
-      </c>
-      <c r="AC7" t="s">
-        <v>123</v>
-      </c>
-      <c r="AD7" t="s">
-        <v>124</v>
-      </c>
-      <c r="AE7" t="s">
-        <v>110</v>
-      </c>
-      <c r="AF7" t="s">
-        <v>110</v>
-      </c>
-      <c r="AG7" t="s">
-        <v>110</v>
-      </c>
-      <c r="AH7" t="s">
-        <v>110</v>
-      </c>
-      <c r="AI7" t="s">
-        <v>110</v>
-      </c>
-      <c r="AJ7" t="s">
-        <v>110</v>
-      </c>
-      <c r="AK7" t="s">
-        <v>110</v>
-      </c>
-      <c r="AL7" t="s">
-        <v>110</v>
-      </c>
-      <c r="AM7" t="s">
-        <v>110</v>
-      </c>
-      <c r="AN7" t="s">
-        <v>110</v>
-      </c>
-      <c r="AO7" t="s">
-        <v>110</v>
-      </c>
-      <c r="AP7" t="s">
-        <v>110</v>
-      </c>
-      <c r="AQ7" t="s">
-        <v>110</v>
-      </c>
-      <c r="AR7" t="s">
-        <v>110</v>
-      </c>
-      <c r="AS7" t="s">
-        <v>110</v>
-      </c>
-      <c r="AT7" t="s">
-        <v>110</v>
-      </c>
-      <c r="AU7" t="s">
-        <v>110</v>
-      </c>
-      <c r="AV7" t="s">
-        <v>110</v>
-      </c>
-      <c r="AW7" t="s">
-        <v>110</v>
-      </c>
-      <c r="AX7" t="s">
-        <v>110</v>
-      </c>
-      <c r="AY7" t="s">
-        <v>110</v>
-      </c>
-      <c r="AZ7" t="s">
-        <v>110</v>
-      </c>
-      <c r="BA7" t="s">
-        <v>110</v>
-      </c>
-      <c r="BB7" t="s">
-        <v>110</v>
-      </c>
-      <c r="BC7" t="s">
-        <v>110</v>
-      </c>
-      <c r="BD7" t="s">
-        <v>110</v>
-      </c>
-      <c r="BE7" t="s">
         <v>110</v>
       </c>
     </row>

</xml_diff>